<commit_message>
corrigindo as animações do botão
</commit_message>
<xml_diff>
--- a/output/teste_processos.xlsx
+++ b/output/teste_processos.xlsx
@@ -499,17 +499,17 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>processo_2</t>
+          <t>processo_3</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>4835245-15.2024.8.01.2832</t>
+          <t>3130687-11.2024.8.01.5042</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 2</t>
+          <t>Nome Aleatório 98</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -518,28 +518,28 @@
         </is>
       </c>
       <c r="E2" s="3" t="n">
-        <v>12723</v>
+        <v>43679</v>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>25/5/2024</t>
+          <t>7/8/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>processo_3</t>
+          <t>processo_2</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>3130687-11.2024.8.01.5042</t>
+          <t>4835245-15.2024.8.01.2832</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 98</t>
+          <t>Nome Aleatório 2</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -548,11 +548,11 @@
         </is>
       </c>
       <c r="E3" s="3" t="n">
-        <v>43679</v>
+        <v>12723</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>25/5/2024</t>
         </is>
       </c>
     </row>

</xml_diff>